<commit_message>
Created new Status/Source Status Mapping file and links
</commit_message>
<xml_diff>
--- a/analysis/lists-update-202203.xlsx
+++ b/analysis/lists-update-202203.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/new330/cloudstor/Documents/projects/data-management/species-lists/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oco115\PycharmProjects\authoritative-lists\analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="193" documentId="8_{618C1A1D-95F7-C347-B167-AB5952179DC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A541F1C4-2EE8-4490-B689-FC1B1E1C15A1}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{193C3978-F2E8-4361-892F-658A750956F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="54100" yWindow="7720" windowWidth="36120" windowHeight="16120" xr2:uid="{DEC2C309-5344-7B41-9095-947CE26C49D7}"/>
+    <workbookView xWindow="-804" yWindow="5376" windowWidth="21456" windowHeight="13008" xr2:uid="{DEC2C309-5344-7B41-9095-947CE26C49D7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -291,7 +290,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -758,20 +757,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{445F260A-E480-B649-82F9-FCA38A0E53C6}">
   <dimension ref="A2:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="68.875" customWidth="1"/>
-    <col min="2" max="2" width="32.375" customWidth="1"/>
-    <col min="3" max="3" width="62.75" customWidth="1"/>
-    <col min="4" max="4" width="42.75" customWidth="1"/>
+    <col min="1" max="1" width="37" customWidth="1"/>
+    <col min="2" max="2" width="32.3984375" customWidth="1"/>
+    <col min="3" max="3" width="43.59765625" customWidth="1"/>
+    <col min="4" max="4" width="42.69921875" customWidth="1"/>
     <col min="5" max="5" width="33" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" ht="26.1">
+    <row r="2" spans="1:5" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -782,12 +781,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="17.100000000000001" thickBot="1">
+    <row r="3" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="94.5">
+    <row r="4" spans="1:5" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -804,7 +803,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="18" thickBot="1">
+    <row r="5" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>9</v>
       </c>
@@ -812,7 +811,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="16.5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
@@ -829,7 +828,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="47.25">
+    <row r="7" spans="1:5" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>16</v>
       </c>
@@ -843,7 +842,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="63">
+    <row r="8" spans="1:5" ht="78" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>20</v>
       </c>
@@ -860,7 +859,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="18" customFormat="1" ht="157.5">
+    <row r="9" spans="1:5" s="18" customFormat="1" ht="156" x14ac:dyDescent="0.3">
       <c r="A9" s="16" t="s">
         <v>25</v>
       </c>
@@ -874,7 +873,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="14" customFormat="1" ht="162">
+    <row r="10" spans="1:5" s="14" customFormat="1" ht="171.6" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>29</v>
       </c>
@@ -888,7 +887,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="18" thickBot="1">
+    <row r="11" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>33</v>
       </c>
@@ -896,17 +895,17 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="26.1">
+    <row r="12" spans="1:5" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A12" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="17.100000000000001" thickBot="1">
+    <row r="13" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="96.75">
+    <row r="14" spans="1:5" ht="109.2" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>36</v>
       </c>
@@ -923,7 +922,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="141.75">
+    <row r="15" spans="1:5" ht="140.4" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>40</v>
       </c>
@@ -940,7 +939,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="141.75">
+    <row r="16" spans="1:5" ht="140.4" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>45</v>
       </c>
@@ -957,7 +956,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="96.75">
+    <row r="17" spans="1:5" ht="109.2" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>50</v>
       </c>
@@ -974,7 +973,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="173.25">
+    <row r="18" spans="1:5" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>53</v>
       </c>
@@ -991,7 +990,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="110.25">
+    <row r="19" spans="1:5" ht="109.2" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>58</v>
       </c>
@@ -1008,7 +1007,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="173.25">
+    <row r="20" spans="1:5" ht="140.4" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>63</v>
       </c>
@@ -1023,7 +1022,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="63">
+    <row r="21" spans="1:5" ht="78" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>66</v>
       </c>
@@ -1034,7 +1033,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="48.75">
+    <row r="22" spans="1:5" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>67</v>
       </c>
@@ -1400,17 +1399,46 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{299CBCC4-ACBA-41EB-8B12-330E35CD4CC1}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{299CBCC4-ACBA-41EB-8B12-330E35CD4CC1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="979888ae-c261-4e89-be96-593c6ec43372"/>
+    <ds:schemaRef ds:uri="72e63c89-cca7-4a76-8691-2dfae7ae4c97"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{81A41A92-0360-4978-977C-432E4E6727C6}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{81A41A92-0360-4978-977C-432E4E6727C6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A6CC241E-8C73-41EC-BB0A-7E7E26BF74EA}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A6CC241E-8C73-41EC-BB0A-7E7E26BF74EA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A8554732-6167-4A51-BD58-C3A59E0FF788}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A8554732-6167-4A51-BD58-C3A59E0FF788}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="979888ae-c261-4e89-be96-593c6ec43372"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Reworked column names - camel case
</commit_message>
<xml_diff>
--- a/analysis/lists-update-202203.xlsx
+++ b/analysis/lists-update-202203.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oco115\PycharmProjects\authoritative-lists\analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{193C3978-F2E8-4361-892F-658A750956F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87B4C34C-2D84-46F1-ACA3-8ECBD67BE784}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-804" yWindow="5376" windowWidth="21456" windowHeight="13008" xr2:uid="{DEC2C309-5344-7B41-9095-947CE26C49D7}"/>
+    <workbookView minimized="1" xWindow="4884" yWindow="0" windowWidth="20316" windowHeight="13800" xr2:uid="{DEC2C309-5344-7B41-9095-947CE26C49D7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -758,19 +758,19 @@
   <dimension ref="A2:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="37" customWidth="1"/>
-    <col min="2" max="2" width="32.3984375" customWidth="1"/>
-    <col min="3" max="3" width="43.59765625" customWidth="1"/>
-    <col min="4" max="4" width="42.69921875" customWidth="1"/>
+    <col min="2" max="2" width="32.375" customWidth="1"/>
+    <col min="3" max="3" width="43.625" customWidth="1"/>
+    <col min="4" max="4" width="42.75" customWidth="1"/>
     <col min="5" max="5" width="33" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:5" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -781,12 +781,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="93.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -803,7 +803,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>9</v>
       </c>
@@ -811,7 +811,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
@@ -828,7 +828,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>16</v>
       </c>
@@ -842,7 +842,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="78" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>20</v>
       </c>
@@ -859,7 +859,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="18" customFormat="1" ht="156" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" s="18" customFormat="1" ht="173.25" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
         <v>25</v>
       </c>
@@ -873,7 +873,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="14" customFormat="1" ht="171.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" s="14" customFormat="1" ht="252" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>29</v>
       </c>
@@ -887,7 +887,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>33</v>
       </c>
@@ -895,17 +895,17 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:5" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A12" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="109.2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>36</v>
       </c>
@@ -922,7 +922,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="140.4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" ht="141.75" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>40</v>
       </c>
@@ -939,7 +939,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="140.4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" ht="141.75" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>45</v>
       </c>
@@ -956,7 +956,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="109.2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>50</v>
       </c>
@@ -973,7 +973,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" ht="189" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>53</v>
       </c>
@@ -990,7 +990,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="109.2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>58</v>
       </c>
@@ -1007,7 +1007,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="140.4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" ht="141.75" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>63</v>
       </c>
@@ -1022,7 +1022,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="78" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>66</v>
       </c>
@@ -1033,7 +1033,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>67</v>
       </c>
@@ -1080,6 +1080,77 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_dlc_DocId xmlns="979888ae-c261-4e89-be96-593c6ec43372">MMVRPYZVETWR-1828124309-9718</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="979888ae-c261-4e89-be96-593c6ec43372">
+      <Url>https://csiroau.sharepoint.com/sites/AtlasofLivingAustralia/_layouts/15/DocIdRedir.aspx?ID=MMVRPYZVETWR-1828124309-9718</Url>
+      <Description>MMVRPYZVETWR-1828124309-9718</Description>
+    </_dlc_DocIdUrl>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008061FEDEAAD6264EB33292EA5D421433" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2cf7b329aa2b9537abbdd28305bb0d98">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="979888ae-c261-4e89-be96-593c6ec43372" xmlns:ns3="72e63c89-cca7-4a76-8691-2dfae7ae4c97" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ef94713aeb95317a829d0f53b69773f7" ns2:_="" ns3:_="">
     <xsd:import namespace="979888ae-c261-4e89-be96-593c6ec43372"/>
@@ -1327,78 +1398,33 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A8554732-6167-4A51-BD58-C3A59E0FF788}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="979888ae-c261-4e89-be96-593c6ec43372"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A6CC241E-8C73-41EC-BB0A-7E7E26BF74EA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_dlc_DocId xmlns="979888ae-c261-4e89-be96-593c6ec43372">MMVRPYZVETWR-1828124309-9718</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="979888ae-c261-4e89-be96-593c6ec43372">
-      <Url>https://csiroau.sharepoint.com/sites/AtlasofLivingAustralia/_layouts/15/DocIdRedir.aspx?ID=MMVRPYZVETWR-1828124309-9718</Url>
-      <Description>MMVRPYZVETWR-1828124309-9718</Description>
-    </_dlc_DocIdUrl>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{81A41A92-0360-4978-977C-432E4E6727C6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{299CBCC4-ACBA-41EB-8B12-330E35CD4CC1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1415,30 +1441,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{81A41A92-0360-4978-977C-432E4E6727C6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A6CC241E-8C73-41EC-BB0A-7E7E26BF74EA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A8554732-6167-4A51-BD58-C3A59E0FF788}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="979888ae-c261-4e89-be96-593c6ec43372"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>